<commit_message>
Chat notif pop up , chart report
- change on badge new chat
- change on chart report, deviasi terhadap target untuk client
</commit_message>
<xml_diff>
--- a/1. Dokumen & Literatur/Report Calculation.xlsx
+++ b/1. Dokumen & Literatur/Report Calculation.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\performance-tracking\1. Dokumen &amp; Literatur\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\xampp\htdocs\performance-tracking\1. Dokumen &amp; Literatur\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{047E297B-8310-45E7-99E1-81FE1F5CF375}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E194A25-8A35-45D4-B46A-CBB36F3FB120}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{05208D3B-E17F-44B5-AAFE-C53CB084AF40}"/>
   </bookViews>
@@ -16,24 +16,17 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="timeframe target calc" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="39">
   <si>
     <t>target</t>
   </si>
@@ -144,6 +137,12 @@
   </si>
   <si>
     <t>Kontak Calon Mentor</t>
+  </si>
+  <si>
+    <t>Devisiasi</t>
+  </si>
+  <si>
+    <t>%</t>
   </si>
 </sst>
 </file>
@@ -237,13 +236,13 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="10" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -558,10 +557,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A1C300F-BDCB-4F93-855A-975A21878B92}">
-  <dimension ref="A2:U36"/>
+  <dimension ref="A2:U42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C17" workbookViewId="0">
-      <selection activeCell="Q23" sqref="Q23:Q24"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="K39" sqref="K39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1199,18 +1198,18 @@
         <v>9</v>
       </c>
       <c r="C32">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D32">
         <v>4</v>
       </c>
       <c r="E32">
         <f>(C32/D32)*100</f>
-        <v>75</v>
-      </c>
-      <c r="G32" s="9">
+        <v>25</v>
+      </c>
+      <c r="G32" s="8">
         <f>1-D32/C32</f>
-        <v>-0.33333333333333326</v>
+        <v>-3</v>
       </c>
       <c r="I32">
         <v>6</v>
@@ -1221,7 +1220,7 @@
       <c r="K32">
         <v>7</v>
       </c>
-      <c r="L32" s="10"/>
+      <c r="L32" s="9"/>
       <c r="M32" t="s">
         <v>31</v>
       </c>
@@ -1237,20 +1236,20 @@
         <v>10</v>
       </c>
       <c r="D33">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="E33">
         <f>(D33/C33)*100</f>
-        <v>100</v>
-      </c>
-      <c r="G33" s="9">
+        <v>0</v>
+      </c>
+      <c r="G33" s="8">
         <f>D33/C33-1</f>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="K33">
         <v>5</v>
       </c>
-      <c r="L33" s="11"/>
+      <c r="L33" s="10"/>
       <c r="M33" t="s">
         <v>29</v>
       </c>
@@ -1262,7 +1261,7 @@
       <c r="K34">
         <v>10</v>
       </c>
-      <c r="L34" s="12"/>
+      <c r="L34" s="11"/>
       <c r="M34" t="s">
         <v>30</v>
       </c>
@@ -1273,6 +1272,64 @@
     <row r="36" spans="2:14" x14ac:dyDescent="0.3">
       <c r="D36" t="s">
         <v>14</v>
+      </c>
+    </row>
+    <row r="40" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="C40" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F40" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="41" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B41" t="s">
+        <v>9</v>
+      </c>
+      <c r="C41">
+        <v>1</v>
+      </c>
+      <c r="D41">
+        <v>4</v>
+      </c>
+      <c r="E41">
+        <f>(C41/D41)*100</f>
+        <v>25</v>
+      </c>
+      <c r="F41">
+        <f>E41-100</f>
+        <v>-75</v>
+      </c>
+      <c r="G41" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="42" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B42" t="s">
+        <v>10</v>
+      </c>
+      <c r="C42">
+        <v>10</v>
+      </c>
+      <c r="D42">
+        <v>8</v>
+      </c>
+      <c r="E42">
+        <f>(D42/C42)*100</f>
+        <v>80</v>
+      </c>
+      <c r="F42">
+        <f>E42-100</f>
+        <v>-20</v>
+      </c>
+      <c r="G42" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -1300,20 +1357,20 @@
       <c r="A4" s="7"/>
       <c r="B4" s="7"/>
       <c r="C4" s="7"/>
-      <c r="D4" s="8" t="s">
+      <c r="D4" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="E4" s="8"/>
-      <c r="F4" s="8"/>
-      <c r="G4" s="8"/>
-      <c r="H4" s="8"/>
-      <c r="I4" s="8"/>
-      <c r="J4" s="8"/>
-      <c r="K4" s="8"/>
-      <c r="L4" s="8"/>
-      <c r="M4" s="8"/>
-      <c r="N4" s="8"/>
-      <c r="O4" s="8"/>
+      <c r="E4" s="12"/>
+      <c r="F4" s="12"/>
+      <c r="G4" s="12"/>
+      <c r="H4" s="12"/>
+      <c r="I4" s="12"/>
+      <c r="J4" s="12"/>
+      <c r="K4" s="12"/>
+      <c r="L4" s="12"/>
+      <c r="M4" s="12"/>
+      <c r="N4" s="12"/>
+      <c r="O4" s="12"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">

</xml_diff>